<commit_message>
Agregando conclusiones finales modelamiento predictivo
</commit_message>
<xml_diff>
--- a/Datos130Adecuada.xlsx
+++ b/Datos130Adecuada.xlsx
@@ -1,26 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebas\Desktop\U\Repos\MODELAMIENTO-TMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F06DE0-1DB7-4FEC-A9AC-4DBDAE49CEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDDC1C7-B8B4-4879-A11A-895B212C01F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$AM$127</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3692" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3690" uniqueCount="188">
   <si>
     <t>DI</t>
   </si>
@@ -490,9 +506,6 @@
     <t>43679740</t>
   </si>
   <si>
-    <t>98488071</t>
-  </si>
-  <si>
     <t>43620593</t>
   </si>
   <si>
@@ -575,9 +588,6 @@
   </si>
   <si>
     <t>43414454</t>
-  </si>
-  <si>
-    <t>1,116E+09</t>
   </si>
   <si>
     <t>42878155</t>
@@ -625,8 +635,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -925,11 +936,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -2633,7 +2646,7 @@
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
         <v>50</v>
@@ -2871,7 +2884,7 @@
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
@@ -3109,7 +3122,7 @@
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B19" t="s">
         <v>50</v>
@@ -3704,7 +3717,7 @@
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B24" t="s">
         <v>50</v>
@@ -3755,7 +3768,7 @@
         <v>44</v>
       </c>
       <c r="R24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S24" t="s">
         <v>46</v>
@@ -3823,7 +3836,7 @@
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
@@ -3942,7 +3955,7 @@
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B26" t="s">
         <v>50</v>
@@ -4774,8 +4787,8 @@
       </c>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>185</v>
+      <c r="A33" s="1">
+        <v>1116000000</v>
       </c>
       <c r="B33" t="s">
         <v>40</v>
@@ -4812,6 +4825,9 @@
       </c>
       <c r="M33">
         <v>3.5</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
       </c>
       <c r="Q33" t="s">
         <v>46</v>
@@ -5123,7 +5139,7 @@
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B36" t="s">
         <v>50</v>
@@ -5174,7 +5190,7 @@
         <v>44</v>
       </c>
       <c r="R36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S36" t="s">
         <v>44</v>
@@ -5242,7 +5258,7 @@
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B37" t="s">
         <v>50</v>
@@ -5956,7 +5972,7 @@
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B43" t="s">
         <v>40</v>
@@ -6075,7 +6091,7 @@
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B44" t="s">
         <v>40</v>
@@ -6126,7 +6142,7 @@
         <v>44</v>
       </c>
       <c r="R44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S44" t="s">
         <v>46</v>
@@ -6789,7 +6805,7 @@
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B50" t="s">
         <v>50</v>
@@ -7859,8 +7875,8 @@
       </c>
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>156</v>
+      <c r="A59">
+        <v>98488071</v>
       </c>
       <c r="B59" t="s">
         <v>40</v>
@@ -7903,6 +7919,9 @@
       </c>
       <c r="O59">
         <v>0.85</v>
+      </c>
+      <c r="P59">
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="Q59" t="s">
         <v>46</v>
@@ -7976,7 +7995,7 @@
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B60" t="s">
         <v>50</v>
@@ -8452,7 +8471,7 @@
     </row>
     <row r="64" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B64" t="s">
         <v>50</v>
@@ -8690,7 +8709,7 @@
     </row>
     <row r="66" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B66" t="s">
         <v>40</v>
@@ -9401,7 +9420,7 @@
     </row>
     <row r="72" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B72" t="s">
         <v>40</v>
@@ -9877,7 +9896,7 @@
     </row>
     <row r="76" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B76" t="s">
         <v>40</v>
@@ -10115,7 +10134,7 @@
     </row>
     <row r="78" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B78" t="s">
         <v>40</v>
@@ -10285,7 +10304,7 @@
         <v>44</v>
       </c>
       <c r="R79" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="S79" t="s">
         <v>46</v>
@@ -11067,7 +11086,7 @@
     </row>
     <row r="86" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B86" t="s">
         <v>40</v>
@@ -11305,7 +11324,7 @@
     </row>
     <row r="88" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B88" t="s">
         <v>50</v>
@@ -11662,7 +11681,7 @@
     </row>
     <row r="91" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B91" t="s">
         <v>40</v>
@@ -11900,7 +11919,7 @@
     </row>
     <row r="93" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B93" t="s">
         <v>40</v>
@@ -12138,7 +12157,7 @@
     </row>
     <row r="95" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B95" t="s">
         <v>50</v>
@@ -12376,7 +12395,7 @@
     </row>
     <row r="97" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B97" t="s">
         <v>40</v>
@@ -12495,7 +12514,7 @@
     </row>
     <row r="98" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B98" t="s">
         <v>40</v>
@@ -12852,7 +12871,7 @@
     </row>
     <row r="101" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B101" t="s">
         <v>40</v>
@@ -13209,7 +13228,7 @@
     </row>
     <row r="104" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B104" t="s">
         <v>40</v>
@@ -14280,7 +14299,7 @@
     </row>
     <row r="113" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B113" t="s">
         <v>40</v>
@@ -14399,7 +14418,7 @@
     </row>
     <row r="114" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B114" t="s">
         <v>50</v>
@@ -14875,7 +14894,7 @@
     </row>
     <row r="118" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B118" t="s">
         <v>50</v>
@@ -15351,7 +15370,7 @@
     </row>
     <row r="122" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B122" t="s">
         <v>50</v>
@@ -15708,7 +15727,7 @@
     </row>
     <row r="125" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B125" t="s">
         <v>40</v>
@@ -16064,6 +16083,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AM127" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AM127">
     <sortCondition ref="E7:E127"/>
   </sortState>

</xml_diff>